<commit_message>
Add feature: generate excel templates of registers.
</commit_message>
<xml_diff>
--- a/excel/templates/template_cn.xlsx
+++ b/excel/templates/template_cn.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hj-micro\regslv\parser\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hj-micro\regslv\parser\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C46836-3EB3-4F28-834C-F4DA5DBF0576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8144D9B-4F1A-416C-87AB-FD1A6FB8A771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="4980" windowWidth="24408" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="3252" windowWidth="22776" windowHeight="13512" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEM" sheetId="1" r:id="rId1"/>
@@ -271,20 +271,6 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>描述</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
       <t>可选值</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -683,6 +669,10 @@
       </rPr>
       <t>]</t>
     </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -795,16 +785,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -815,6 +799,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1103,249 +1099,247 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="18.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="38.77734375" style="3" customWidth="1"/>
-    <col min="4" max="7" width="18.77734375" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="2" width="18.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.77734375" style="2" customWidth="1"/>
+    <col min="4" max="7" width="18.77734375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="8">
         <v>32</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="8"/>
+      <c r="C16" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1359,5 +1353,6 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refine format of code, comments and excel templates
</commit_message>
<xml_diff>
--- a/excel/templates/template_cn.xlsx
+++ b/excel/templates/template_cn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hj-micro\regslv\parser\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A69F9A-BBB3-4C97-A10B-16A395D0A8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FA6761-D5B3-416C-A667-091EACF7D528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="1908" windowWidth="22776" windowHeight="14652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4212" yWindow="1908" windowWidth="22776" windowHeight="14652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEM" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>名称</t>
   </si>
   <si>
-    <t>TEMPLATE寄存器</t>
-  </si>
-  <si>
     <t>地址偏移</t>
   </si>
   <si>
@@ -151,6 +148,10 @@
   </si>
   <si>
     <t>0X00000000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEM</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -582,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -592,10 +593,10 @@
     </row>
     <row r="2" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -605,7 +606,7 @@
     </row>
     <row r="3" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="11">
         <v>32</v>
@@ -618,10 +619,10 @@
     </row>
     <row r="4" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>4</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -631,10 +632,10 @@
     </row>
     <row r="5" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>6</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -644,140 +645,140 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>